<commit_message>
🔄 synced local 'matlabfilesuk/' with remote 'matlabMfilesUK/'
</commit_message>
<xml_diff>
--- a/matlabfilesuk/ch11PCA/washers.xlsx
+++ b/matlabfilesuk/ch11PCA/washers.xlsx
@@ -8,13 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\books\DataScienceWithMatlab\matlabMfilesUK\ch11PCA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C1D7518-E6D5-4E67-A979-F4063925125D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{945BE4D5-D370-4C3F-A7C4-FFDB43475D11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="testo" sheetId="2" r:id="rId1"/>
-    <sheet name="data" sheetId="1" r:id="rId2"/>
+    <sheet name="data" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -420,26 +419,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Foglio1"/>
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>